<commit_message>
Version Finale pour le Benin
</commit_message>
<xml_diff>
--- a/Benin/Admin1.xlsx
+++ b/Benin/Admin1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="379">
   <si>
     <t xml:space="preserve">ASSORTIMENT : Quels sont les prouits Habituellement vendus/UOASoldGroup_Gr/Produits Alimentaires de Céréales</t>
   </si>
@@ -792,6 +792,461 @@
   </si>
   <si>
     <t xml:space="preserve">PRIX  : Quels autres produits non alimentaires n'estimeriez-vous pas correctement/UOAPriceUnstab_NF/Autres produits non alimentaires: ${UOASoldGroup_NF_oth}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : /D1.1 Considérant la demande actuelle de vos clients, votre stock actuel vous permet-il d'y répondre pendant 1 semaine?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : /D1.2 Si vous commandez chez votre fournisseur aujourd'hui, pensez-vous recevoir vos produits en semaine?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : La majorité de vos fournisseurs se trouvent-ils dans la même zone géographique pour/TrdResilNodDens_Gr/Produits Alimentaires de Céréales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : La majorité de vos fournisseurs se trouvent-ils dans la même zone géographique pour/TrdResilNodDens_Gr/Produits Alimentaires - Autres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : La majorité de vos fournisseurs se trouvent-ils dans la même zone géographique pour/TrdResilNodDens_Gr/Produits Non alimentaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : La majorité de vos fournisseurs se trouvent-ils dans la même zone géographique pour/TrdResilNodDens_Gr/N/A - Aucun de ce qui précède</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits Alimentaires de céréales la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FCer/Riz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits Alimentaires de céréales la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FCer/Maïs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits Alimentaires de céréales la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FCer/Manioc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits Alimentaires de céréales la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FCer/Blé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits Alimentaires de céréales la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FCer/Farine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits Alimentaires de céréales la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FCer/Pâtes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits Alimentaires de céréales la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FCer/Pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits Alimentaires de céréales la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FCer/Sorgho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits Alimentaires de céréales la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FCer/Millet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits Alimentaires de céréales la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FCer/Orge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits Alimentaires de céréales la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FCer/Autres aliments de céréales: ${UOASoldGroup_FCer_oth}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels autres produits Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FOth/Racines et tubercules (p. ex. manioc, pommes de terre, igname, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels autres produits Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FOth/Légumineuses, noix et graines (p. ex. haricots, pois, lentilles, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels autres produits Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FOth/Fruits et légumes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels autres produits Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FOth/Lait et produits laitiers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels autres produits Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FOth/Viande, poisson et œufs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels autres produits Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FOth/Huiles et graisses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels autres produits Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FOth/Herbes, condiments et épices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels autres produits Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_FOth/Autres aliments: ${UOASoldGroup_FOth_oth}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_NF/HYGIENE - Eau potable, Tablettes de purification d'eau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_NF/HYGIENE - Matériaux de construction de latrines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_NF/HYGIENE - Produits non Alimentaires d'hygiène (papier toilette, brosse à dents, dentifrice, détergent à lessive, détergent à vaisselle liquide, serviettes hygiéniques, savon individuel)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_NF/Santé - Médecine (Produits pharmaceutiques en vente libre)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_NF/Abri - Articles d'abri (tentes, bâches en plastique, tôle métallique, bâche, abris temporaires, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_NF/Abri - Matériaux de construction (bricks, bambou, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_NF/Maison - Vêtements incluant les chaussures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_NF/Maison - Literie (filets de lit, Couverture, tapis de sol/matelas, isolation au sol, moustiquaires)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_NF/Maison - Ustensiles de cuisine et couverts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_NF/Maison - Autres poêles, carburant et éclairage (p. ex. GPL, gaz, bois de chauffage, charbon de bois, solaire)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_NF/Éducation - Matériel scolaire (Livres scolaires, crayons, Uniformes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_NF/Communication - Téléphones mobiles/cartes/services SIM et Internet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non Alimentaires la plupart de vos fournisseurs sont-ils
+ géographiquement situés au même endroit?/TrdResilNodDens_NF/Autres produits non alimentaires: ${UOASoldGroup_NF_oth}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Avez-vous actuellement plus d'un fournisseur pour:/TrdResilNodComplex_Gr/Produits Alimentaires de Céréales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Avez-vous actuellement plus d'un fournisseur pour:/TrdResilNodComplex_Gr/Produits Alimentaires - Autres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Avez-vous actuellement plus d'un fournisseur pour:/TrdResilNodComplex_Gr/Produits Non alimentaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Avez-vous actuellement plus d'un fournisseur pour:/TrdResilNodComplex_Gr/N/A - Aucun de ce qui précède</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits alimentaires de céréals avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FCer/Riz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits alimentaires de céréals avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FCer/Maïs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits alimentaires de céréals avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FCer/Manioc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits alimentaires de céréals avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FCer/Blé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits alimentaires de céréals avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FCer/Farine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits alimentaires de céréals avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FCer/Pâtes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits alimentaires de céréals avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FCer/Pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits alimentaires de céréals avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FCer/Sorgho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits alimentaires de céréals avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FCer/Millet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits alimentaires de céréals avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FCer/Orge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits alimentaires de céréals avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FCer/Autres aliments de céréales: ${UOASoldGroup_FCer_oth}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels autres produits produits avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FOth/Racines et tubercules (p. ex. manioc, pommes de terre, igname, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels autres produits produits avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FOth/Légumineuses, noix et graines (p. ex. haricots, pois, lentilles, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels autres produits produits avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FOth/Fruits et légumes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels autres produits produits avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FOth/Lait et produits laitiers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels autres produits produits avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FOth/Viande, poisson et œufs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels autres produits produits avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FOth/Huiles et graisses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels autres produits produits avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FOth/Herbes, condiments et épices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels autres produits produits avez-vous actuellement UN SEUL (1)
+ fournisseur?:/TrdResilNodComplex_FOth/Autres aliments: ${UOASoldGroup_FOth_oth}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non alimentaires avez-vous actuellement UN SEUL (1)
+ fournisseur?/TrdResilNodComplex_NF/HYGIENE - Eau potable, Tablettes de purification d'eau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non alimentaires avez-vous actuellement UN SEUL (1)
+ fournisseur?/TrdResilNodComplex_NF/HYGIENE - Matériaux de construction de latrines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non alimentaires avez-vous actuellement UN SEUL (1)
+ fournisseur?/TrdResilNodComplex_NF/HYGIENE - Produits non Alimentaires d'hygiène (papier toilette, brosse à dents, dentifrice, détergent à lessive, détergent à vaisselle liquide, serviettes hygiéniques, savon individuel)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non alimentaires avez-vous actuellement UN SEUL (1)
+ fournisseur?/TrdResilNodComplex_NF/Santé - Médecine (Produits pharmaceutiques en vente libre)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non alimentaires avez-vous actuellement UN SEUL (1)
+ fournisseur?/TrdResilNodComplex_NF/Abri - Articles d'abri (tentes, bâches en plastique, tôle métallique, bâche, abris temporaires, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non alimentaires avez-vous actuellement UN SEUL (1)
+ fournisseur?/TrdResilNodComplex_NF/Abri - Matériaux de construction (bricks, bambou, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non alimentaires avez-vous actuellement UN SEUL (1)
+ fournisseur?/TrdResilNodComplex_NF/Maison - Vêtements incluant les chaussures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non alimentaires avez-vous actuellement UN SEUL (1)
+ fournisseur?/TrdResilNodComplex_NF/Maison - Literie (filets de lit, Couverture, tapis de sol/matelas, isolation au sol, moustiquaires)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non alimentaires avez-vous actuellement UN SEUL (1)
+ fournisseur?/TrdResilNodComplex_NF/Maison - Ustensiles de cuisine et couverts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non alimentaires avez-vous actuellement UN SEUL (1)
+ fournisseur?/TrdResilNodComplex_NF/Maison - Autres poêles, carburant et éclairage (p. ex. GPL, gaz, bois de chauffage, charbon de bois, solaire)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non alimentaires avez-vous actuellement UN SEUL (1)
+ fournisseur?/TrdResilNodComplex_NF/Éducation - Matériel scolaire (Livres scolaires, crayons, Uniformes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non alimentaires avez-vous actuellement UN SEUL (1)
+ fournisseur?/TrdResilNodComplex_NF/Communication - Téléphones mobiles/cartes/services SIM et Internet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisement, pour quels produits non alimentaires avez-vous actuellement UN SEUL (1)
+ fournisseur?/TrdResilNodComplex_NF/Autres produits non alimentaires: ${UOASoldGroup_NF_oth}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Votre entreprise compte-t-elle principalement sur un seul fournisseur pour:/TrdResilNodCrit_Gr/Produits Alimentaires de Céréales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Votre entreprise compte-t-elle principalement sur un seul fournisseur pour:/TrdResilNodCrit_Gr/Produits Alimentaires - Autres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Votre entreprise compte-t-elle principalement sur un seul fournisseur pour:/TrdResilNodCrit_Gr/Produits Non alimentaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Votre entreprise compte-t-elle principalement sur un seul fournisseur pour:/TrdResilNodCrit_Gr/N/A - Aucun de ce qui précède</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits alimentaires de céréales existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FCer/Riz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits alimentaires de céréales existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FCer/Maïs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits alimentaires de céréales existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FCer/Manioc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits alimentaires de céréales existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FCer/Blé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits alimentaires de céréales existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FCer/Farine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits alimentaires de céréales existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FCer/Pâtes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits alimentaires de céréales existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FCer/Pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits alimentaires de céréales existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FCer/Sorgho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits alimentaires de céréales existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FCer/Millet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits alimentaires de céréales existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FCer/Orge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits alimentaires de céréales existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FCer/Autres aliments de céréales: ${UOASoldGroup_FCer_oth}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels autres produits alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FOth/Racines et tubercules (p. ex. manioc, pommes de terre, igname, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels autres produits alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FOth/Légumineuses, noix et graines (p. ex. haricots, pois, lentilles, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels autres produits alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FOth/Fruits et légumes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels autres produits alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FOth/Lait et produits laitiers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels autres produits alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FOth/Viande, poisson et œufs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels autres produits alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FOth/Huiles et graisses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels autres produits alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FOth/Herbes, condiments et épices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels autres produits alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_FOth/Autres aliments: ${UOASoldGroup_FOth_oth}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits non alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_NF/HYGIENE - Eau potable, Tablettes de purification d'eau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits non alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_NF/HYGIENE - Matériaux de construction de latrines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits non alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_NF/HYGIENE - Produits non Alimentaires d'hygiène (papier toilette, brosse à dents, dentifrice, détergent à lessive, détergent à vaisselle liquide, serviettes hygiéniques, savon individuel)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits non alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_NF/Santé - Médecine (Produits pharmaceutiques en vente libre)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits non alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_NF/Abri - Articles d'abri (tentes, bâches en plastique, tôle métallique, bâche, abris temporaires, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits non alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_NF/Abri - Matériaux de construction (bricks, bambou, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits non alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_NF/Maison - Vêtements incluant les chaussures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits non alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_NF/Maison - Literie (filets de lit, Couverture, tapis de sol/matelas, isolation au sol, moustiquaires)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits non alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_NF/Maison - Ustensiles de cuisine et couverts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits non alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_NF/Maison - Autres poêles, carburant et éclairage (p. ex. GPL, gaz, bois de chauffage, charbon de bois, solaire)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits non alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_NF/Éducation - Matériel scolaire (Livres scolaires, crayons, Uniformes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits non alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_NF/Communication - Téléphones mobiles/cartes/services SIM et Internet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESILIENCE  : Plus précisément, pour quels produits non alimentaires existe-t-il un seul fournisseur de qui dépend la
+ plupart de votre entreprise?:/TrdResilNodCrit_NF/Autres produits non alimentaires: ${UOASoldGroup_NF_oth}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERVICE : TrdServiceLoyalty Offrez-vous un programme de fidélité à vos clients réguliers? Réductions ou système de
+ points à utiliser plus tard dans votre boutique?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERVICE : Cette boutique possède-t-elle un terminal de vente (POS)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERVICE : Analysez-vous les informations collectées par votre terminal de vente. Informations du
+  type, inventaire, catalogue de données?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99</t>
   </si>
 </sst>
 </file>
@@ -7219,6 +7674,3579 @@
         <v>83</v>
       </c>
     </row>
+    <row r="753">
+      <c r="A753" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="s">
+        <v>1</v>
+      </c>
+      <c r="B754" t="s">
+        <v>2</v>
+      </c>
+      <c r="C754" t="s">
+        <v>3</v>
+      </c>
+      <c r="D754" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="s">
+        <v>5</v>
+      </c>
+      <c r="B755" t="s">
+        <v>111</v>
+      </c>
+      <c r="C755" t="s">
+        <v>135</v>
+      </c>
+      <c r="D755" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="s">
+        <v>1</v>
+      </c>
+      <c r="B758" t="s">
+        <v>2</v>
+      </c>
+      <c r="C758" t="s">
+        <v>3</v>
+      </c>
+      <c r="D758" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="s">
+        <v>5</v>
+      </c>
+      <c r="B759" t="s">
+        <v>39</v>
+      </c>
+      <c r="C759" t="s">
+        <v>239</v>
+      </c>
+      <c r="D759" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="s">
+        <v>1</v>
+      </c>
+      <c r="B762" t="s">
+        <v>2</v>
+      </c>
+      <c r="C762" t="s">
+        <v>3</v>
+      </c>
+      <c r="D762" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="s">
+        <v>5</v>
+      </c>
+      <c r="B763" t="s">
+        <v>34</v>
+      </c>
+      <c r="C763" t="s">
+        <v>49</v>
+      </c>
+      <c r="D763" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="s">
+        <v>1</v>
+      </c>
+      <c r="B766" t="s">
+        <v>2</v>
+      </c>
+      <c r="C766" t="s">
+        <v>3</v>
+      </c>
+      <c r="D766" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="s">
+        <v>5</v>
+      </c>
+      <c r="B767" t="s">
+        <v>34</v>
+      </c>
+      <c r="C767" t="s">
+        <v>49</v>
+      </c>
+      <c r="D767" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="s">
+        <v>1</v>
+      </c>
+      <c r="B770" t="s">
+        <v>2</v>
+      </c>
+      <c r="C770" t="s">
+        <v>3</v>
+      </c>
+      <c r="D770" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="s">
+        <v>5</v>
+      </c>
+      <c r="B771" t="s">
+        <v>178</v>
+      </c>
+      <c r="C771" t="s">
+        <v>88</v>
+      </c>
+      <c r="D771" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="s">
+        <v>1</v>
+      </c>
+      <c r="B774" t="s">
+        <v>2</v>
+      </c>
+      <c r="C774" t="s">
+        <v>3</v>
+      </c>
+      <c r="D774" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="s">
+        <v>5</v>
+      </c>
+      <c r="B775" t="s">
+        <v>239</v>
+      </c>
+      <c r="C775" t="s">
+        <v>39</v>
+      </c>
+      <c r="D775" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="s">
+        <v>1</v>
+      </c>
+      <c r="B778" t="s">
+        <v>2</v>
+      </c>
+      <c r="C778" t="s">
+        <v>3</v>
+      </c>
+      <c r="D778" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="s">
+        <v>5</v>
+      </c>
+      <c r="B779" t="s">
+        <v>123</v>
+      </c>
+      <c r="C779" t="s">
+        <v>47</v>
+      </c>
+      <c r="D779" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="s">
+        <v>1</v>
+      </c>
+      <c r="B782" t="s">
+        <v>2</v>
+      </c>
+      <c r="C782" t="s">
+        <v>3</v>
+      </c>
+      <c r="D782" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="s">
+        <v>5</v>
+      </c>
+      <c r="B783" t="s">
+        <v>59</v>
+      </c>
+      <c r="C783" t="s">
+        <v>101</v>
+      </c>
+      <c r="D783" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="s">
+        <v>1</v>
+      </c>
+      <c r="B786" t="s">
+        <v>2</v>
+      </c>
+      <c r="C786" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="s">
+        <v>5</v>
+      </c>
+      <c r="B787" t="s">
+        <v>49</v>
+      </c>
+      <c r="C787" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="s">
+        <v>1</v>
+      </c>
+      <c r="B790" t="s">
+        <v>2</v>
+      </c>
+      <c r="C790" t="s">
+        <v>3</v>
+      </c>
+      <c r="D790" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="s">
+        <v>5</v>
+      </c>
+      <c r="B791" t="s">
+        <v>46</v>
+      </c>
+      <c r="C791" t="s">
+        <v>8</v>
+      </c>
+      <c r="D791" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="s">
+        <v>1</v>
+      </c>
+      <c r="B794" t="s">
+        <v>2</v>
+      </c>
+      <c r="C794" t="s">
+        <v>3</v>
+      </c>
+      <c r="D794" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="s">
+        <v>5</v>
+      </c>
+      <c r="B795" t="s">
+        <v>17</v>
+      </c>
+      <c r="C795" t="s">
+        <v>24</v>
+      </c>
+      <c r="D795" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="s">
+        <v>1</v>
+      </c>
+      <c r="B798" t="s">
+        <v>2</v>
+      </c>
+      <c r="C798" t="s">
+        <v>3</v>
+      </c>
+      <c r="D798" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="s">
+        <v>5</v>
+      </c>
+      <c r="B799" t="s">
+        <v>67</v>
+      </c>
+      <c r="C799" t="s">
+        <v>69</v>
+      </c>
+      <c r="D799" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="s">
+        <v>1</v>
+      </c>
+      <c r="B802" t="s">
+        <v>2</v>
+      </c>
+      <c r="C802" t="s">
+        <v>3</v>
+      </c>
+      <c r="D802" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="s">
+        <v>5</v>
+      </c>
+      <c r="B803" t="s">
+        <v>38</v>
+      </c>
+      <c r="C803" t="s">
+        <v>42</v>
+      </c>
+      <c r="D803" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="s">
+        <v>1</v>
+      </c>
+      <c r="B806" t="s">
+        <v>2</v>
+      </c>
+      <c r="C806" t="s">
+        <v>3</v>
+      </c>
+      <c r="D806" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="s">
+        <v>5</v>
+      </c>
+      <c r="B807" t="s">
+        <v>111</v>
+      </c>
+      <c r="C807" t="s">
+        <v>50</v>
+      </c>
+      <c r="D807" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="s">
+        <v>1</v>
+      </c>
+      <c r="B810" t="s">
+        <v>2</v>
+      </c>
+      <c r="C810" t="s">
+        <v>3</v>
+      </c>
+      <c r="D810" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="s">
+        <v>5</v>
+      </c>
+      <c r="B811" t="s">
+        <v>31</v>
+      </c>
+      <c r="C811" t="s">
+        <v>81</v>
+      </c>
+      <c r="D811" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="s">
+        <v>1</v>
+      </c>
+      <c r="B814" t="s">
+        <v>2</v>
+      </c>
+      <c r="C814" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="s">
+        <v>5</v>
+      </c>
+      <c r="B815" t="s">
+        <v>49</v>
+      </c>
+      <c r="C815" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="s">
+        <v>1</v>
+      </c>
+      <c r="B818" t="s">
+        <v>2</v>
+      </c>
+      <c r="C818" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="s">
+        <v>5</v>
+      </c>
+      <c r="B819" t="s">
+        <v>49</v>
+      </c>
+      <c r="C819" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="s">
+        <v>1</v>
+      </c>
+      <c r="B822" t="s">
+        <v>2</v>
+      </c>
+      <c r="C822" t="s">
+        <v>3</v>
+      </c>
+      <c r="D822" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="s">
+        <v>5</v>
+      </c>
+      <c r="B823" t="s">
+        <v>38</v>
+      </c>
+      <c r="C823" t="s">
+        <v>121</v>
+      </c>
+      <c r="D823" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="s">
+        <v>1</v>
+      </c>
+      <c r="B826" t="s">
+        <v>2</v>
+      </c>
+      <c r="C826" t="s">
+        <v>3</v>
+      </c>
+      <c r="D826" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="s">
+        <v>5</v>
+      </c>
+      <c r="B827" t="s">
+        <v>73</v>
+      </c>
+      <c r="C827" t="s">
+        <v>55</v>
+      </c>
+      <c r="D827" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="s">
+        <v>1</v>
+      </c>
+      <c r="B830" t="s">
+        <v>2</v>
+      </c>
+      <c r="C830" t="s">
+        <v>3</v>
+      </c>
+      <c r="D830" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="s">
+        <v>5</v>
+      </c>
+      <c r="B831" t="s">
+        <v>53</v>
+      </c>
+      <c r="C831" t="s">
+        <v>107</v>
+      </c>
+      <c r="D831" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="s">
+        <v>1</v>
+      </c>
+      <c r="B834" t="s">
+        <v>2</v>
+      </c>
+      <c r="C834" t="s">
+        <v>3</v>
+      </c>
+      <c r="D834" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="s">
+        <v>5</v>
+      </c>
+      <c r="B835" t="s">
+        <v>47</v>
+      </c>
+      <c r="C835" t="s">
+        <v>123</v>
+      </c>
+      <c r="D835" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="s">
+        <v>1</v>
+      </c>
+      <c r="B838" t="s">
+        <v>2</v>
+      </c>
+      <c r="C838" t="s">
+        <v>3</v>
+      </c>
+      <c r="D838" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="s">
+        <v>5</v>
+      </c>
+      <c r="B839" t="s">
+        <v>38</v>
+      </c>
+      <c r="C839" t="s">
+        <v>42</v>
+      </c>
+      <c r="D839" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="s">
+        <v>1</v>
+      </c>
+      <c r="B842" t="s">
+        <v>2</v>
+      </c>
+      <c r="C842" t="s">
+        <v>3</v>
+      </c>
+      <c r="D842" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="s">
+        <v>5</v>
+      </c>
+      <c r="B843" t="s">
+        <v>32</v>
+      </c>
+      <c r="C843" t="s">
+        <v>32</v>
+      </c>
+      <c r="D843" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="s">
+        <v>1</v>
+      </c>
+      <c r="B846" t="s">
+        <v>2</v>
+      </c>
+      <c r="C846" t="s">
+        <v>3</v>
+      </c>
+      <c r="D846" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="s">
+        <v>5</v>
+      </c>
+      <c r="B847" t="s">
+        <v>32</v>
+      </c>
+      <c r="C847" t="s">
+        <v>32</v>
+      </c>
+      <c r="D847" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="s">
+        <v>1</v>
+      </c>
+      <c r="B850" t="s">
+        <v>2</v>
+      </c>
+      <c r="C850" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="s">
+        <v>5</v>
+      </c>
+      <c r="B851" t="s">
+        <v>49</v>
+      </c>
+      <c r="C851" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="s">
+        <v>1</v>
+      </c>
+      <c r="B854" t="s">
+        <v>2</v>
+      </c>
+      <c r="C854" t="s">
+        <v>3</v>
+      </c>
+      <c r="D854" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="s">
+        <v>5</v>
+      </c>
+      <c r="B855" t="s">
+        <v>73</v>
+      </c>
+      <c r="C855" t="s">
+        <v>121</v>
+      </c>
+      <c r="D855" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="s">
+        <v>1</v>
+      </c>
+      <c r="B858" t="s">
+        <v>2</v>
+      </c>
+      <c r="C858" t="s">
+        <v>3</v>
+      </c>
+      <c r="D858" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="s">
+        <v>5</v>
+      </c>
+      <c r="B859" t="s">
+        <v>201</v>
+      </c>
+      <c r="C859" t="s">
+        <v>24</v>
+      </c>
+      <c r="D859" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="s">
+        <v>1</v>
+      </c>
+      <c r="B862" t="s">
+        <v>2</v>
+      </c>
+      <c r="C862" t="s">
+        <v>3</v>
+      </c>
+      <c r="D862" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="s">
+        <v>5</v>
+      </c>
+      <c r="B863" t="s">
+        <v>39</v>
+      </c>
+      <c r="C863" t="s">
+        <v>50</v>
+      </c>
+      <c r="D863" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="s">
+        <v>1</v>
+      </c>
+      <c r="B866" t="s">
+        <v>2</v>
+      </c>
+      <c r="C866" t="s">
+        <v>3</v>
+      </c>
+      <c r="D866" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="s">
+        <v>5</v>
+      </c>
+      <c r="B867" t="s">
+        <v>73</v>
+      </c>
+      <c r="C867" t="s">
+        <v>121</v>
+      </c>
+      <c r="D867" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="s">
+        <v>1</v>
+      </c>
+      <c r="B870" t="s">
+        <v>2</v>
+      </c>
+      <c r="C870" t="s">
+        <v>3</v>
+      </c>
+      <c r="D870" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="s">
+        <v>5</v>
+      </c>
+      <c r="B871" t="s">
+        <v>136</v>
+      </c>
+      <c r="C871" t="s">
+        <v>65</v>
+      </c>
+      <c r="D871" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="s">
+        <v>1</v>
+      </c>
+      <c r="B874" t="s">
+        <v>2</v>
+      </c>
+      <c r="C874" t="s">
+        <v>3</v>
+      </c>
+      <c r="D874" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="s">
+        <v>5</v>
+      </c>
+      <c r="B875" t="s">
+        <v>21</v>
+      </c>
+      <c r="C875" t="s">
+        <v>24</v>
+      </c>
+      <c r="D875" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="s">
+        <v>1</v>
+      </c>
+      <c r="B878" t="s">
+        <v>2</v>
+      </c>
+      <c r="C878" t="s">
+        <v>3</v>
+      </c>
+      <c r="D878" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="s">
+        <v>5</v>
+      </c>
+      <c r="B879" t="s">
+        <v>47</v>
+      </c>
+      <c r="C879" t="s">
+        <v>69</v>
+      </c>
+      <c r="D879" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="s">
+        <v>1</v>
+      </c>
+      <c r="B882" t="s">
+        <v>2</v>
+      </c>
+      <c r="C882" t="s">
+        <v>3</v>
+      </c>
+      <c r="D882" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="s">
+        <v>5</v>
+      </c>
+      <c r="B883" t="s">
+        <v>201</v>
+      </c>
+      <c r="C883" t="s">
+        <v>24</v>
+      </c>
+      <c r="D883" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="s">
+        <v>1</v>
+      </c>
+      <c r="B886" t="s">
+        <v>2</v>
+      </c>
+      <c r="C886" t="s">
+        <v>3</v>
+      </c>
+      <c r="D886" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="s">
+        <v>5</v>
+      </c>
+      <c r="B887" t="s">
+        <v>111</v>
+      </c>
+      <c r="C887" t="s">
+        <v>107</v>
+      </c>
+      <c r="D887" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="s">
+        <v>1</v>
+      </c>
+      <c r="B890" t="s">
+        <v>2</v>
+      </c>
+      <c r="C890" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="s">
+        <v>5</v>
+      </c>
+      <c r="B891" t="s">
+        <v>88</v>
+      </c>
+      <c r="C891" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="s">
+        <v>1</v>
+      </c>
+      <c r="B894" t="s">
+        <v>2</v>
+      </c>
+      <c r="C894" t="s">
+        <v>3</v>
+      </c>
+      <c r="D894" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="s">
+        <v>5</v>
+      </c>
+      <c r="B895" t="s">
+        <v>20</v>
+      </c>
+      <c r="C895" t="s">
+        <v>81</v>
+      </c>
+      <c r="D895" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="s">
+        <v>1</v>
+      </c>
+      <c r="B898" t="s">
+        <v>2</v>
+      </c>
+      <c r="C898" t="s">
+        <v>3</v>
+      </c>
+      <c r="D898" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="s">
+        <v>5</v>
+      </c>
+      <c r="B899" t="s">
+        <v>21</v>
+      </c>
+      <c r="C899" t="s">
+        <v>24</v>
+      </c>
+      <c r="D899" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="s">
+        <v>1</v>
+      </c>
+      <c r="B902" t="s">
+        <v>2</v>
+      </c>
+      <c r="C902" t="s">
+        <v>3</v>
+      </c>
+      <c r="D902" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="s">
+        <v>5</v>
+      </c>
+      <c r="B903" t="s">
+        <v>21</v>
+      </c>
+      <c r="C903" t="s">
+        <v>24</v>
+      </c>
+      <c r="D903" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="s">
+        <v>1</v>
+      </c>
+      <c r="B906" t="s">
+        <v>2</v>
+      </c>
+      <c r="C906" t="s">
+        <v>3</v>
+      </c>
+      <c r="D906" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="s">
+        <v>5</v>
+      </c>
+      <c r="B907" t="s">
+        <v>178</v>
+      </c>
+      <c r="C907" t="s">
+        <v>88</v>
+      </c>
+      <c r="D907" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="s">
+        <v>1</v>
+      </c>
+      <c r="B910" t="s">
+        <v>2</v>
+      </c>
+      <c r="C910" t="s">
+        <v>3</v>
+      </c>
+      <c r="D910" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="s">
+        <v>5</v>
+      </c>
+      <c r="B911" t="s">
+        <v>7</v>
+      </c>
+      <c r="C911" t="s">
+        <v>53</v>
+      </c>
+      <c r="D911" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="s">
+        <v>1</v>
+      </c>
+      <c r="B914" t="s">
+        <v>2</v>
+      </c>
+      <c r="C914" t="s">
+        <v>3</v>
+      </c>
+      <c r="D914" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="s">
+        <v>5</v>
+      </c>
+      <c r="B915" t="s">
+        <v>178</v>
+      </c>
+      <c r="C915" t="s">
+        <v>88</v>
+      </c>
+      <c r="D915" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="s">
+        <v>1</v>
+      </c>
+      <c r="B918" t="s">
+        <v>2</v>
+      </c>
+      <c r="C918" t="s">
+        <v>3</v>
+      </c>
+      <c r="D918" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="s">
+        <v>5</v>
+      </c>
+      <c r="B919" t="s">
+        <v>302</v>
+      </c>
+      <c r="C919" t="s">
+        <v>47</v>
+      </c>
+      <c r="D919" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="s">
+        <v>1</v>
+      </c>
+      <c r="B922" t="s">
+        <v>2</v>
+      </c>
+      <c r="C922" t="s">
+        <v>3</v>
+      </c>
+      <c r="D922" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="s">
+        <v>5</v>
+      </c>
+      <c r="B923" t="s">
+        <v>81</v>
+      </c>
+      <c r="C923" t="s">
+        <v>27</v>
+      </c>
+      <c r="D923" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="s">
+        <v>1</v>
+      </c>
+      <c r="B926" t="s">
+        <v>2</v>
+      </c>
+      <c r="C926" t="s">
+        <v>3</v>
+      </c>
+      <c r="D926" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="s">
+        <v>5</v>
+      </c>
+      <c r="B927" t="s">
+        <v>27</v>
+      </c>
+      <c r="C927" t="s">
+        <v>81</v>
+      </c>
+      <c r="D927" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="s">
+        <v>1</v>
+      </c>
+      <c r="B930" t="s">
+        <v>2</v>
+      </c>
+      <c r="C930" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="s">
+        <v>5</v>
+      </c>
+      <c r="B931" t="s">
+        <v>50</v>
+      </c>
+      <c r="C931" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="s">
+        <v>1</v>
+      </c>
+      <c r="B934" t="s">
+        <v>2</v>
+      </c>
+      <c r="C934" t="s">
+        <v>3</v>
+      </c>
+      <c r="D934" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="s">
+        <v>5</v>
+      </c>
+      <c r="B935" t="s">
+        <v>50</v>
+      </c>
+      <c r="C935" t="s">
+        <v>42</v>
+      </c>
+      <c r="D935" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="s">
+        <v>1</v>
+      </c>
+      <c r="B938" t="s">
+        <v>2</v>
+      </c>
+      <c r="C938" t="s">
+        <v>3</v>
+      </c>
+      <c r="D938" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="s">
+        <v>5</v>
+      </c>
+      <c r="B939" t="s">
+        <v>50</v>
+      </c>
+      <c r="C939" t="s">
+        <v>42</v>
+      </c>
+      <c r="D939" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="s">
+        <v>1</v>
+      </c>
+      <c r="B942" t="s">
+        <v>2</v>
+      </c>
+      <c r="C942" t="s">
+        <v>3</v>
+      </c>
+      <c r="D942" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="s">
+        <v>5</v>
+      </c>
+      <c r="B943" t="s">
+        <v>69</v>
+      </c>
+      <c r="C943" t="s">
+        <v>65</v>
+      </c>
+      <c r="D943" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="s">
+        <v>1</v>
+      </c>
+      <c r="B946" t="s">
+        <v>2</v>
+      </c>
+      <c r="C946" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="s">
+        <v>5</v>
+      </c>
+      <c r="B947" t="s">
+        <v>50</v>
+      </c>
+      <c r="C947" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="s">
+        <v>1</v>
+      </c>
+      <c r="B950" t="s">
+        <v>2</v>
+      </c>
+      <c r="C950" t="s">
+        <v>3</v>
+      </c>
+      <c r="D950" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="s">
+        <v>5</v>
+      </c>
+      <c r="B951" t="s">
+        <v>29</v>
+      </c>
+      <c r="C951" t="s">
+        <v>24</v>
+      </c>
+      <c r="D951" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="s">
+        <v>1</v>
+      </c>
+      <c r="B954" t="s">
+        <v>2</v>
+      </c>
+      <c r="C954" t="s">
+        <v>3</v>
+      </c>
+      <c r="D954" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="s">
+        <v>5</v>
+      </c>
+      <c r="B955" t="s">
+        <v>50</v>
+      </c>
+      <c r="C955" t="s">
+        <v>42</v>
+      </c>
+      <c r="D955" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="s">
+        <v>1</v>
+      </c>
+      <c r="B958" t="s">
+        <v>2</v>
+      </c>
+      <c r="C958" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="s">
+        <v>5</v>
+      </c>
+      <c r="B959" t="s">
+        <v>50</v>
+      </c>
+      <c r="C959" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="s">
+        <v>1</v>
+      </c>
+      <c r="B962" t="s">
+        <v>2</v>
+      </c>
+      <c r="C962" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="s">
+        <v>5</v>
+      </c>
+      <c r="B963" t="s">
+        <v>50</v>
+      </c>
+      <c r="C963" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="s">
+        <v>1</v>
+      </c>
+      <c r="B966" t="s">
+        <v>2</v>
+      </c>
+      <c r="C966" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="s">
+        <v>5</v>
+      </c>
+      <c r="B967" t="s">
+        <v>50</v>
+      </c>
+      <c r="C967" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="s">
+        <v>1</v>
+      </c>
+      <c r="B970" t="s">
+        <v>2</v>
+      </c>
+      <c r="C970" t="s">
+        <v>3</v>
+      </c>
+      <c r="D970" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="s">
+        <v>5</v>
+      </c>
+      <c r="B971" t="s">
+        <v>29</v>
+      </c>
+      <c r="C971" t="s">
+        <v>24</v>
+      </c>
+      <c r="D971" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="s">
+        <v>1</v>
+      </c>
+      <c r="B974" t="s">
+        <v>2</v>
+      </c>
+      <c r="C974" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="s">
+        <v>5</v>
+      </c>
+      <c r="B975" t="s">
+        <v>50</v>
+      </c>
+      <c r="C975" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="s">
+        <v>1</v>
+      </c>
+      <c r="B978" t="s">
+        <v>2</v>
+      </c>
+      <c r="C978" t="s">
+        <v>3</v>
+      </c>
+      <c r="D978" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="s">
+        <v>5</v>
+      </c>
+      <c r="B979" t="s">
+        <v>69</v>
+      </c>
+      <c r="C979" t="s">
+        <v>8</v>
+      </c>
+      <c r="D979" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="s">
+        <v>1</v>
+      </c>
+      <c r="B982" t="s">
+        <v>2</v>
+      </c>
+      <c r="C982" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="s">
+        <v>5</v>
+      </c>
+      <c r="B983" t="s">
+        <v>50</v>
+      </c>
+      <c r="C983" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="s">
+        <v>1</v>
+      </c>
+      <c r="B986" t="s">
+        <v>2</v>
+      </c>
+      <c r="C986" t="s">
+        <v>3</v>
+      </c>
+      <c r="D986" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="s">
+        <v>5</v>
+      </c>
+      <c r="B987" t="s">
+        <v>69</v>
+      </c>
+      <c r="C987" t="s">
+        <v>8</v>
+      </c>
+      <c r="D987" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="s">
+        <v>1</v>
+      </c>
+      <c r="B990" t="s">
+        <v>2</v>
+      </c>
+      <c r="C990" t="s">
+        <v>3</v>
+      </c>
+      <c r="D990" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="s">
+        <v>5</v>
+      </c>
+      <c r="B991" t="s">
+        <v>65</v>
+      </c>
+      <c r="C991" t="s">
+        <v>69</v>
+      </c>
+      <c r="D991" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="s">
+        <v>1</v>
+      </c>
+      <c r="B994" t="s">
+        <v>2</v>
+      </c>
+      <c r="C994" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="s">
+        <v>5</v>
+      </c>
+      <c r="B995" t="s">
+        <v>50</v>
+      </c>
+      <c r="C995" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="s">
+        <v>1</v>
+      </c>
+      <c r="B998" t="s">
+        <v>2</v>
+      </c>
+      <c r="C998" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="s">
+        <v>5</v>
+      </c>
+      <c r="B999" t="s">
+        <v>75</v>
+      </c>
+      <c r="C999" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1006" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1007" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1011" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1014" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1015" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1018" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1019" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1019" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1022" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1022" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1023" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1023" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1026" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1026" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1026" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1027" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1027" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1027" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1030" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1030" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1030" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1031" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1031" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1031" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1034" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1034" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1035" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1035" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1038" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1038" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1038" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1039" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1039" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1039" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1042" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1042" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1043" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1043" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1046" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1046" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1046" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1047" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1047" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1047" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1050" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1050" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1050" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1051" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1051" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1051" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1054" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1054" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1054" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1055" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1055" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1055" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1058" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1058" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1058" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1059" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1059" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1059" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1062" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1062" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1062" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1063" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1063" t="s">
+        <v>341</v>
+      </c>
+      <c r="D1063" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1066" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1066" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1066" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1067" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1067" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1067" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1070" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1070" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1070" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1071" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1071" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1071" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1074" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1074" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1075" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1075" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1078" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1078" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1078" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1079" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1079" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1079" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1082" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1082" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1082" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1083" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1083" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1083" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1086" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1086" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1086" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1087" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1087" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1087" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1090" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1090" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1090" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1091" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1091" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1091" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1094" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1094" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1094" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1095" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1095" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1095" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1098" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1098" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1098" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1099" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1099" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1099" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1102" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1102" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1103" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1103" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1106" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1106" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1107" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1107" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1110" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1110" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1110" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1111" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1111" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1111" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1114" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1114" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1114" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1115" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1115" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1115" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1118" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1118" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1118" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1119" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1119" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1119" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1122" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1122" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1122" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1123" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1123" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1123" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1126" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1126" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1126" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1127" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1127" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1127" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1130" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1130" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1130" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1131" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1131" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1131" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1134" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1134" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1134" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1135" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1135" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1135" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1138" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1138" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1139" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1139" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1142" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1142" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1142" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1143" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1143" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1143" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1146" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1146" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1146" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1147" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1147" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1147" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1150" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1150" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1150" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1151" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1151" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1151" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1154" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1154" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1154" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1155" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1155" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1155" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1158" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1158" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1158" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1159" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1159" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1159" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1162" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1162" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1163" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1163" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1166" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1166" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1166" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1167" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1167" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1167" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1170" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1170" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1170" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1171" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1171" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1171" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1174" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1174" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1174" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1175" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1175" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1175" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1178" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1178" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1178" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1179" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1179" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1179" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1182" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1182" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1182" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1183" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1183" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1183" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1186" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1186" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1186" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1187" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1187" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1187" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1190" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1190" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1190" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1191" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1191" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1191" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1194" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1194" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1194" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1195" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1195" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1195" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1198" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1198" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1198" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1199" t="s">
+        <v>304</v>
+      </c>
+      <c r="C1199" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1199" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1202" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1202" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1203" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1203" t="s">
+        <v>378</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>